<commit_message>
Licences are exported as numbers instead of strings now
This allows for formatting to be done in the excel file, which give more flexibility
</commit_message>
<xml_diff>
--- a/webroot/resources/ab-llr-template.xlsx
+++ b/webroot/resources/ab-llr-template.xlsx
@@ -1158,12 +1158,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="00"/>
     <numFmt numFmtId="166" formatCode="000"/>
-    <numFmt numFmtId="167" formatCode="0000000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1396,7 +1395,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1463,11 +1462,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1486,7 +1480,14 @@
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0000000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1820,9 +1821,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1838,7 +1841,7 @@
     <col min="10" max="10" width="6.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" style="25" customWidth="1"/>
     <col min="12" max="12" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1848,24 +1851,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>355</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="43"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="40"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O3" s="16" t="s">
@@ -1982,7 +1985,7 @@
       <c r="L7" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="M7" s="38" t="s">
+      <c r="M7" s="27" t="s">
         <v>175</v>
       </c>
       <c r="N7" s="10" t="s">
@@ -2068,7 +2071,7 @@
       <c r="L8" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="26" t="s">
         <v>326</v>
       </c>
       <c r="N8" s="7" t="s">
@@ -2110,6 +2113,612 @@
       <c r="Z8" s="8" t="s">
         <v>339</v>
       </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M9" s="26"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M10" s="26"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M12" s="26"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M14" s="26"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M15" s="26"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M16" s="26"/>
+    </row>
+    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="26"/>
+    </row>
+    <row r="20" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="26"/>
+    </row>
+    <row r="22" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="26"/>
+    </row>
+    <row r="23" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="26"/>
+    </row>
+    <row r="24" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="26"/>
+    </row>
+    <row r="25" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="26"/>
+    </row>
+    <row r="26" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="26"/>
+    </row>
+    <row r="27" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="26"/>
+    </row>
+    <row r="28" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="26"/>
+    </row>
+    <row r="29" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="26"/>
+    </row>
+    <row r="30" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="26"/>
+    </row>
+    <row r="31" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M31" s="26"/>
+    </row>
+    <row r="32" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M32" s="26"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="26"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="26"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="26"/>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M36" s="26"/>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M37" s="26"/>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M38" s="26"/>
+    </row>
+    <row r="39" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M39" s="26"/>
+    </row>
+    <row r="40" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M40" s="26"/>
+    </row>
+    <row r="41" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M41" s="26"/>
+    </row>
+    <row r="42" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="26"/>
+    </row>
+    <row r="43" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="26"/>
+    </row>
+    <row r="44" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M44" s="26"/>
+    </row>
+    <row r="45" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M45" s="26"/>
+    </row>
+    <row r="46" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M46" s="26"/>
+    </row>
+    <row r="47" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M47" s="26"/>
+    </row>
+    <row r="48" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="26"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M49" s="26"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="26"/>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M51" s="26"/>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M52" s="26"/>
+    </row>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M53" s="26"/>
+    </row>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M54" s="26"/>
+    </row>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M55" s="26"/>
+    </row>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M56" s="26"/>
+    </row>
+    <row r="57" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M57" s="26"/>
+    </row>
+    <row r="58" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M58" s="26"/>
+    </row>
+    <row r="59" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M59" s="26"/>
+    </row>
+    <row r="60" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M60" s="26"/>
+    </row>
+    <row r="61" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M61" s="26"/>
+    </row>
+    <row r="62" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M62" s="26"/>
+    </row>
+    <row r="63" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M63" s="26"/>
+    </row>
+    <row r="64" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M64" s="26"/>
+    </row>
+    <row r="65" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M65" s="26"/>
+    </row>
+    <row r="66" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M66" s="26"/>
+    </row>
+    <row r="67" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M67" s="26"/>
+    </row>
+    <row r="68" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M68" s="26"/>
+    </row>
+    <row r="69" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M69" s="26"/>
+    </row>
+    <row r="70" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M70" s="26"/>
+    </row>
+    <row r="71" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M71" s="26"/>
+    </row>
+    <row r="72" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M72" s="26"/>
+    </row>
+    <row r="73" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M73" s="26"/>
+    </row>
+    <row r="74" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M74" s="26"/>
+    </row>
+    <row r="75" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M75" s="26"/>
+    </row>
+    <row r="76" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M76" s="26"/>
+    </row>
+    <row r="77" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M77" s="26"/>
+    </row>
+    <row r="78" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M78" s="26"/>
+    </row>
+    <row r="79" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M79" s="26"/>
+    </row>
+    <row r="80" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M80" s="26"/>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M81" s="26"/>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M82" s="26"/>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M83" s="26"/>
+    </row>
+    <row r="84" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M84" s="26"/>
+    </row>
+    <row r="85" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M85" s="26"/>
+    </row>
+    <row r="86" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M86" s="26"/>
+    </row>
+    <row r="87" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M87" s="26"/>
+    </row>
+    <row r="88" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M88" s="26"/>
+    </row>
+    <row r="89" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M89" s="26"/>
+    </row>
+    <row r="90" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M90" s="26"/>
+    </row>
+    <row r="91" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M91" s="26"/>
+    </row>
+    <row r="92" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M92" s="26"/>
+    </row>
+    <row r="93" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M93" s="26"/>
+    </row>
+    <row r="94" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M94" s="26"/>
+    </row>
+    <row r="95" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M95" s="26"/>
+    </row>
+    <row r="96" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M96" s="26"/>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M97" s="26"/>
+    </row>
+    <row r="98" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M98" s="26"/>
+    </row>
+    <row r="99" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M99" s="26"/>
+    </row>
+    <row r="100" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M100" s="26"/>
+    </row>
+    <row r="101" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M101" s="26"/>
+    </row>
+    <row r="102" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M102" s="26"/>
+    </row>
+    <row r="103" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M103" s="26"/>
+    </row>
+    <row r="104" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M104" s="26"/>
+    </row>
+    <row r="105" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M105" s="26"/>
+    </row>
+    <row r="106" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M106" s="26"/>
+    </row>
+    <row r="107" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M107" s="26"/>
+    </row>
+    <row r="108" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M108" s="26"/>
+    </row>
+    <row r="109" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M109" s="26"/>
+    </row>
+    <row r="110" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M110" s="26"/>
+    </row>
+    <row r="111" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M111" s="26"/>
+    </row>
+    <row r="112" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M112" s="26"/>
+    </row>
+    <row r="113" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M113" s="26"/>
+    </row>
+    <row r="114" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M114" s="26"/>
+    </row>
+    <row r="115" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M115" s="26"/>
+    </row>
+    <row r="116" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M116" s="26"/>
+    </row>
+    <row r="117" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M117" s="26"/>
+    </row>
+    <row r="118" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M118" s="26"/>
+    </row>
+    <row r="119" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M119" s="26"/>
+    </row>
+    <row r="120" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M120" s="26"/>
+    </row>
+    <row r="121" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M121" s="26"/>
+    </row>
+    <row r="122" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M122" s="26"/>
+    </row>
+    <row r="123" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M123" s="26"/>
+    </row>
+    <row r="124" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M124" s="26"/>
+    </row>
+    <row r="125" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M125" s="26"/>
+    </row>
+    <row r="126" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M126" s="26"/>
+    </row>
+    <row r="127" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M127" s="26"/>
+    </row>
+    <row r="128" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M128" s="26"/>
+    </row>
+    <row r="129" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M129" s="26"/>
+    </row>
+    <row r="130" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M130" s="26"/>
+    </row>
+    <row r="131" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M131" s="26"/>
+    </row>
+    <row r="132" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M132" s="26"/>
+    </row>
+    <row r="133" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M133" s="26"/>
+    </row>
+    <row r="134" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M134" s="26"/>
+    </row>
+    <row r="135" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M135" s="26"/>
+    </row>
+    <row r="136" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M136" s="26"/>
+    </row>
+    <row r="137" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M137" s="26"/>
+    </row>
+    <row r="138" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M138" s="26"/>
+    </row>
+    <row r="139" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M139" s="26"/>
+    </row>
+    <row r="140" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M140" s="26"/>
+    </row>
+    <row r="141" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M141" s="26"/>
+    </row>
+    <row r="142" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M142" s="26"/>
+    </row>
+    <row r="143" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M143" s="26"/>
+    </row>
+    <row r="144" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M144" s="26"/>
+    </row>
+    <row r="145" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M145" s="26"/>
+    </row>
+    <row r="146" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M146" s="26"/>
+    </row>
+    <row r="147" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M147" s="26"/>
+    </row>
+    <row r="148" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M148" s="26"/>
+    </row>
+    <row r="149" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M149" s="26"/>
+    </row>
+    <row r="150" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M150" s="26"/>
+    </row>
+    <row r="151" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M151" s="26"/>
+    </row>
+    <row r="152" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M152" s="26"/>
+    </row>
+    <row r="153" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M153" s="26"/>
+    </row>
+    <row r="154" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M154" s="26"/>
+    </row>
+    <row r="155" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M155" s="26"/>
+    </row>
+    <row r="156" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M156" s="26"/>
+    </row>
+    <row r="157" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M157" s="26"/>
+    </row>
+    <row r="158" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M158" s="26"/>
+    </row>
+    <row r="159" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M159" s="26"/>
+    </row>
+    <row r="160" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M160" s="26"/>
+    </row>
+    <row r="161" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M161" s="26"/>
+    </row>
+    <row r="162" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M162" s="26"/>
+    </row>
+    <row r="163" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M163" s="26"/>
+    </row>
+    <row r="164" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M164" s="26"/>
+    </row>
+    <row r="165" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M165" s="26"/>
+    </row>
+    <row r="166" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M166" s="26"/>
+    </row>
+    <row r="167" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M167" s="26"/>
+    </row>
+    <row r="168" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M168" s="26"/>
+    </row>
+    <row r="169" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M169" s="26"/>
+    </row>
+    <row r="170" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M170" s="26"/>
+    </row>
+    <row r="171" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M171" s="26"/>
+    </row>
+    <row r="172" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M172" s="26"/>
+    </row>
+    <row r="173" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M173" s="26"/>
+    </row>
+    <row r="174" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M174" s="26"/>
+    </row>
+    <row r="175" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M175" s="26"/>
+    </row>
+    <row r="176" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M176" s="26"/>
+    </row>
+    <row r="177" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M177" s="26"/>
+    </row>
+    <row r="178" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M178" s="26"/>
+    </row>
+    <row r="179" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M179" s="26"/>
+    </row>
+    <row r="180" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M180" s="26"/>
+    </row>
+    <row r="181" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M181" s="26"/>
+    </row>
+    <row r="182" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M182" s="26"/>
+    </row>
+    <row r="183" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M183" s="26"/>
+    </row>
+    <row r="184" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M184" s="26"/>
+    </row>
+    <row r="185" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M185" s="26"/>
+    </row>
+    <row r="186" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M186" s="26"/>
+    </row>
+    <row r="187" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M187" s="26"/>
+    </row>
+    <row r="188" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M188" s="26"/>
+    </row>
+    <row r="189" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M189" s="26"/>
+    </row>
+    <row r="190" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M190" s="26"/>
+    </row>
+    <row r="191" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M191" s="26"/>
+    </row>
+    <row r="192" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M192" s="26"/>
+    </row>
+    <row r="193" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M193" s="26"/>
+    </row>
+    <row r="194" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M194" s="26"/>
+    </row>
+    <row r="195" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M195" s="26"/>
+    </row>
+    <row r="196" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M196" s="26"/>
+    </row>
+    <row r="197" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M197" s="26"/>
+    </row>
+    <row r="198" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M198" s="26"/>
+    </row>
+    <row r="199" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M199" s="26"/>
+    </row>
+    <row r="200" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M200" s="26"/>
+    </row>
+    <row r="201" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M201" s="26"/>
+    </row>
+    <row r="202" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M202" s="26"/>
+    </row>
+    <row r="203" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M203" s="26"/>
+    </row>
+    <row r="204" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M204" s="26"/>
+    </row>
+    <row r="205" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M205" s="26"/>
+    </row>
+    <row r="206" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M206" s="26"/>
+    </row>
+    <row r="207" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M207" s="26"/>
+    </row>
+    <row r="208" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M208" s="26"/>
+    </row>
+    <row r="209" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M209" s="26"/>
+    </row>
+    <row r="210" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M210" s="26"/>
     </row>
   </sheetData>
   <autoFilter ref="A7:Z8"/>

</xml_diff>